<commit_message>
Add bulk upload functionality with test data and template
- Created `sankha-bulk-test-v2.xlsx` for testing bulk uploads with sample product data.
- Implemented `generate_test_bulk.js` to generate an Excel file with various product scenarios, including perfect, partial, minimal, broken, and missing required data.
- Developed `sankha-bulk-template-script.js` to create a template for bulk uploads with detailed instructions for users.
- Added `test-bulk-upload-missing-fields.xlsx` to test cases with missing fields in the product data.
</commit_message>
<xml_diff>
--- a/test-bulk-upload.xlsx
+++ b/test-bulk-upload.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -397,32 +398,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="60.83203125" customWidth="1"/>
+    <col min="9" max="9" width="60.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
         <v>Product Name</v>
       </c>
       <c r="B1" t="str">
+        <v>Category</v>
+      </c>
+      <c r="C1" t="str">
         <v>Brand</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>SKU</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Base Price (MWK)</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Stock Quantity</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Condition</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>Description</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Specs (JSON)</v>
       </c>
     </row>
     <row r="2">
@@ -430,22 +448,28 @@
         <v>iPhone 15 Pro Max 256GB</v>
       </c>
       <c r="B2" t="str">
+        <v>Smartphones</v>
+      </c>
+      <c r="C2" t="str">
         <v>Apple</v>
       </c>
-      <c r="C2" t="str">
-        <v>SKU-IP15PM-001</v>
-      </c>
-      <c r="D2">
-        <v>450000</v>
+      <c r="D2" t="str">
+        <v>IP15PM-256-BLK</v>
       </c>
       <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2" t="str">
+        <v>1500000</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="str">
         <v>NEW</v>
       </c>
-      <c r="G2" t="str">
-        <v>Latest iPhone with titanium design</v>
+      <c r="H2" t="str">
+        <v>Brand new, sealed in box. 1 year warranty.</v>
+      </c>
+      <c r="I2" t="str">
+        <v>{"storage":"256GB","color":"Black Titanium","ram":"8GB"}</v>
       </c>
     </row>
     <row r="3">
@@ -453,211 +477,120 @@
         <v>Samsung Galaxy S24 Ultra</v>
       </c>
       <c r="B3" t="str">
+        <v>Smartphones</v>
+      </c>
+      <c r="C3" t="str">
         <v>Samsung</v>
       </c>
-      <c r="C3" t="str">
-        <v>SKU-SGS24U-001</v>
-      </c>
-      <c r="D3">
-        <v>380000</v>
+      <c r="D3" t="str">
+        <v>SGS24U-512-GRY</v>
       </c>
       <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3" t="str">
+        <v>1350000</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="str">
         <v>NEW</v>
       </c>
-      <c r="G3" t="str">
-        <v>Flagship Samsung with S Pen</v>
+      <c r="H3" t="str">
+        <v>Factory unlocked. Includes S Pen.</v>
+      </c>
+      <c r="I3" t="str">
+        <v>{"storage":"512GB","color":"Titanium Gray","ram":"12GB"}</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="120.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>BULK UPLOAD INSTRUCTIONS</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Required Columns:</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>MacBook Air M3 13-inch</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Apple</v>
-      </c>
-      <c r="C4" t="str">
-        <v>SKU-MBA-M3-001</v>
-      </c>
-      <c r="D4">
-        <v>750000</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Lightweight laptop with M3 chip</v>
+        <v>- Product Name: The name of the product</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Sony WH-1000XM5 Headphones</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Sony</v>
-      </c>
-      <c r="C5" t="str">
-        <v>SKU-SONY-XM5</v>
-      </c>
-      <c r="D5">
-        <v>120000</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Premium noise cancelling headphones</v>
+        <v>- Base Price (MWK): Your selling price BEFORE platform fees</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>iPad Pro 12.9 M2</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Apple</v>
-      </c>
-      <c r="C6" t="str">
-        <v>SKU-IPAD-PRO</v>
-      </c>
-      <c r="D6">
-        <v>620000</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6" t="str">
-        <v>REFURBISHED</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Refurbished iPad Pro in excellent condition</v>
+        <v>- Stock Quantity: Number of items in stock</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Dell XPS 15 Laptop</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Dell</v>
-      </c>
-      <c r="C7" t="str">
-        <v>SKU-DELL-XPS15</v>
-      </c>
-      <c r="D7">
-        <v>890000</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="G7" t="str">
-        <v>15-inch premium Windows laptop</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>AirPods Pro 2nd Gen</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Apple</v>
-      </c>
-      <c r="C8" t="str">
-        <v>SKU-APP2-001</v>
-      </c>
-      <c r="D8">
-        <v>95000</v>
-      </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
-      <c r="F8" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="G8" t="str">
-        <v>Wireless earbuds with active noise cancellation</v>
+        <v>Optional Columns:</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Samsung 55 inch OLED TV</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Samsung</v>
-      </c>
-      <c r="C9" t="str">
-        <v>SKU-SAM-TV55</v>
-      </c>
-      <c r="D9">
-        <v>520000</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="G9" t="str">
-        <v>4K OLED Smart TV</v>
+        <v>- Category, Brand, SKU, Condition, Description, Specs (JSON)</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Logitech MX Master 3S Mouse</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Logitech</v>
-      </c>
-      <c r="C10" t="str">
-        <v>SKU-LOG-MX3S</v>
-      </c>
-      <c r="D10">
-        <v>45000</v>
-      </c>
-      <c r="E10">
-        <v>20</v>
-      </c>
-      <c r="F10" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="G10" t="str">
-        <v>Premium wireless mouse</v>
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>JBL Charge 5 Speaker</v>
-      </c>
-      <c r="B11" t="str">
-        <v>JBL</v>
-      </c>
-      <c r="C11" t="str">
-        <v>SKU-JBL-CH5</v>
-      </c>
-      <c r="D11">
-        <v>65000</v>
-      </c>
-      <c r="E11">
-        <v>12</v>
-      </c>
-      <c r="F11" t="str">
-        <v>USED_LIKE_NEW</v>
-      </c>
-      <c r="G11" t="str">
-        <v>Portable Bluetooth speaker</v>
+        <v>Notes:</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>- Remove sample rows before uploading real products</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>- Max 200 products per upload</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>- Prices are in MWK</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>